<commit_message>
fix sheet name in marian_plum and column in mango
</commit_message>
<xml_diff>
--- a/Backend/predict_py/data.xlsx
+++ b/Backend/predict_py/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kmitlthailand-my.sharepoint.com/personal/63050671_kmitl_ac_th/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ipin0\Downloads\FruitInventorySystem\fis\FIS\Backend\predict_py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{DF17CB99-E0AC-4739-BF24-094BC1A35965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCC895D7-E8D9-44F0-8CA6-217BEEE22434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="10" xr2:uid="{C1739C25-3296-441F-9BD2-A07A7E121FB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="11" xr2:uid="{C1739C25-3296-441F-9BD2-A07A7E121FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="orange" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="avocado" sheetId="8" r:id="rId8"/>
     <sheet name="strawberry" sheetId="9" r:id="rId9"/>
     <sheet name="mangosteen" sheetId="10" r:id="rId10"/>
-    <sheet name="marian plum" sheetId="20" r:id="rId11"/>
+    <sheet name="marian_plum" sheetId="20" r:id="rId11"/>
     <sheet name="mango" sheetId="11" r:id="rId12"/>
     <sheet name="red guava" sheetId="12" r:id="rId13"/>
     <sheet name="spinach" sheetId="13" r:id="rId14"/>
@@ -108,7 +108,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -181,9 +181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีม Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -221,7 +221,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -327,7 +327,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -469,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -483,10 +483,10 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="19.09765625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1042,14 +1042,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD28EEE2-F54B-4A40-B6CC-AD98619616CD}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="17.296875" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1604,14 +1604,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBF7492-982F-428F-95D8-D3E240B38B78}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.69921875" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,558 +2164,606 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E871D3AB-C1BE-4EB1-AE97-62DDF423693B}">
-  <dimension ref="B1:F49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.8984375" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="4" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <v>2563</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2563</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="2">
+      <c r="C14" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="2">
+      <c r="C15" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="2">
+      <c r="C16" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="2">
+      <c r="C17" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="2">
+      <c r="C18" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="2">
+      <c r="C19" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
-        <v>2564</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>2564</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="2">
+      <c r="C27" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="2">
+      <c r="C28" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="2">
+      <c r="C29" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="2">
+      <c r="C30" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="2">
+      <c r="C31" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="2">
+      <c r="C32" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="2">
-        <v>2565</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>2565</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="2">
+      <c r="C38" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="2">
+      <c r="C39" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="2">
+      <c r="C40" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="2">
+      <c r="C41" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="2">
+      <c r="C42" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="2">
+      <c r="C43" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="C45" s="2">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="C46" s="2">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D47" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="2">
-        <v>2566</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>2566</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="2">
-        <v>0</v>
-      </c>
-      <c r="F49" s="3">
-        <f>SUM(D2:D49)</f>
+      <c r="C49" s="2">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="3">
+        <f>SUM(C2:C49)</f>
         <v>234</v>
       </c>
     </row>
@@ -2732,10 +2780,10 @@
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.69921875" customWidth="1"/>
-    <col min="3" max="3" width="17.69921875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3294,10 +3342,10 @@
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.8984375" customWidth="1"/>
-    <col min="3" max="3" width="18.296875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3856,10 +3904,10 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="14.8984375" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4418,9 +4466,9 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4975,14 +5023,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058EE804-5CA8-46DF-B7BD-62675F4030ED}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.296875" customWidth="1"/>
-    <col min="3" max="3" width="16.09765625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5541,10 +5589,10 @@
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="16.796875" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6103,10 +6151,10 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.296875" customWidth="1"/>
-    <col min="3" max="3" width="20.3984375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6665,11 +6713,11 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="17.09765625" customWidth="1"/>
-    <col min="3" max="3" width="19.09765625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7222,16 +7270,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4419DF20-968E-4368-89A8-86C945A55593}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.296875" customWidth="1"/>
-    <col min="3" max="3" width="21.296875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7776,6 +7824,10 @@
         <f>SUM(C2:C49)</f>
         <v>3628</v>
       </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7790,10 +7842,10 @@
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.8984375" customWidth="1"/>
-    <col min="3" max="3" width="19.8984375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -8348,14 +8400,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AA2558-0FD8-42BE-87B8-24CE67960B83}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.296875" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -8914,10 +8966,10 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.796875" customWidth="1"/>
-    <col min="3" max="3" width="23.296875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -9472,14 +9524,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752495F-38AD-414C-B37D-3398987B6F0B}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="16.796875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -10038,10 +10090,10 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="18.09765625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix volume < 0 and change model to sarisma
</commit_message>
<xml_diff>
--- a/Backend/predict_py/data.xlsx
+++ b/Backend/predict_py/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ipin0\Downloads\FruitInventorySystem\fis\FIS\Backend\predict_py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCC895D7-E8D9-44F0-8CA6-217BEEE22434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB997277-DC10-45E2-A73B-DABF50ECC909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="11" xr2:uid="{C1739C25-3296-441F-9BD2-A07A7E121FB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C1739C25-3296-441F-9BD2-A07A7E121FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="orange" sheetId="1" r:id="rId1"/>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7681024-19E6-4AFF-99B0-83A68B7A8A52}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,13 +1042,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD28EEE2-F54B-4A40-B6CC-AD98619616CD}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2166,7 +2166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E871D3AB-C1BE-4EB1-AE97-62DDF423693B}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>

</xml_diff>